<commit_message>
Changing 'cost' to 'quote'
</commit_message>
<xml_diff>
--- a/resources/test_data_user.xlsx
+++ b/resources/test_data_user.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\OneDrive - UNSW\University\Postgraduate\Year 3 Trimester 3\COMP9900\Project\BackEnd\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kovid\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E45687C-0E9A-4CD3-B6CF-C80AC835E545}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6C896FF-1808-4380-875C-C4A8EEC57A06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14880" windowHeight="21000" firstSheet="2" activeTab="6" xr2:uid="{1A28855D-1372-4992-8C97-28705A0C69E1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="2" activeTab="5" xr2:uid="{1A28855D-1372-4992-8C97-28705A0C69E1}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
@@ -215,9 +215,6 @@
     <t>transaction</t>
   </si>
   <si>
-    <t>cost</t>
-  </si>
-  <si>
     <t>trade_type</t>
   </si>
   <si>
@@ -678,6 +675,9 @@
   </si>
   <si>
     <t>HUOBI</t>
+  </si>
+  <si>
+    <t>quote</t>
   </si>
 </sst>
 </file>
@@ -1147,7 +1147,7 @@
         <v>23</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>53</v>
@@ -1158,7 +1158,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -1180,7 +1180,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -1202,7 +1202,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
@@ -1224,7 +1224,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -1246,7 +1246,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C6" t="s">
         <v>14</v>
@@ -1615,7 +1615,7 @@
         <v>42</v>
       </c>
       <c r="C1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D1" t="s">
         <v>53</v>
@@ -1626,7 +1626,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1634,7 +1634,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1642,7 +1642,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1650,7 +1650,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1658,7 +1658,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1775,8 +1775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{839B1F08-9FB4-4205-9D29-58AB9BDB11FE}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A16:E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1796,19 +1796,19 @@
         <v>27</v>
       </c>
       <c r="D1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E1" t="s">
         <v>54</v>
-      </c>
-      <c r="E1" t="s">
-        <v>55</v>
       </c>
       <c r="F1" t="s">
         <v>44</v>
       </c>
       <c r="G1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" t="s">
         <v>56</v>
-      </c>
-      <c r="H1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1825,7 +1825,7 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F2" s="7">
         <v>44119.108414351853</v>
@@ -1851,7 +1851,7 @@
         <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F3" s="7">
         <v>44119.108414351853</v>
@@ -1877,7 +1877,7 @@
         <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F4" s="6">
         <v>44119.108419884258</v>
@@ -1903,7 +1903,7 @@
         <v>40</v>
       </c>
       <c r="E5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F5" s="6">
         <v>44119.108419884258</v>
@@ -1929,7 +1929,7 @@
         <v>50</v>
       </c>
       <c r="E6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F6" s="6">
         <v>44119.108419884258</v>
@@ -1955,7 +1955,7 @@
         <v>60</v>
       </c>
       <c r="E7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F7" s="7">
         <v>44119.108414351853</v>
@@ -1981,7 +1981,7 @@
         <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F8" s="7">
         <v>44119.233414351853</v>
@@ -2007,7 +2007,7 @@
         <v>20</v>
       </c>
       <c r="E9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F9" s="7">
         <v>44119.275081018517</v>
@@ -2033,7 +2033,7 @@
         <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F10" s="7">
         <v>44119.441747685189</v>
@@ -2059,7 +2059,7 @@
         <v>20</v>
       </c>
       <c r="E11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F11" s="7">
         <v>44119.441747685189</v>
@@ -2085,7 +2085,7 @@
         <v>30</v>
       </c>
       <c r="E12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F12" s="7">
         <v>44119.441747685189</v>
@@ -2111,7 +2111,7 @@
         <v>40</v>
       </c>
       <c r="E13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F13" s="7">
         <v>44119.441747685189</v>
@@ -2137,7 +2137,7 @@
         <v>30</v>
       </c>
       <c r="E14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F14" s="7">
         <v>44119.441747685189</v>
@@ -2163,7 +2163,7 @@
         <v>40</v>
       </c>
       <c r="E15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F15" s="7">
         <v>44119.441747685189</v>
@@ -2189,7 +2189,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F16" s="7">
         <v>44119.441747685189</v>
@@ -2215,7 +2215,7 @@
         <v>20</v>
       </c>
       <c r="E17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F17" s="7">
         <v>44119.441747685189</v>
@@ -2241,7 +2241,7 @@
         <v>60</v>
       </c>
       <c r="E18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F18" s="7">
         <v>44119.483414351853</v>
@@ -2267,7 +2267,7 @@
         <v>60</v>
       </c>
       <c r="E19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F19" s="7">
         <v>44119.483414351853</v>
@@ -2293,7 +2293,7 @@
         <v>60</v>
       </c>
       <c r="E20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F20" s="7">
         <v>44119.483414351853</v>
@@ -2319,7 +2319,7 @@
         <v>60</v>
       </c>
       <c r="E21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F21" s="7">
         <v>44119.483414351853</v>
@@ -2353,7 +2353,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB0AE7CC-0281-42AB-BEFB-FF7CDAA66D40}">
   <dimension ref="A1:C76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+    <sheetView topLeftCell="A44" workbookViewId="0">
       <selection activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
@@ -2364,21 +2364,21 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75">
       <c r="A1" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75">
       <c r="A2" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>70</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>71</v>
       </c>
       <c r="C2" t="b">
         <v>0</v>
@@ -2386,10 +2386,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.75">
       <c r="A3" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>72</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>73</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
@@ -2397,10 +2397,10 @@
     </row>
     <row r="4" spans="1:3" ht="15.75">
       <c r="A4" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>74</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>75</v>
       </c>
       <c r="C4" t="b">
         <v>0</v>
@@ -2408,10 +2408,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75">
       <c r="A5" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>76</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>77</v>
       </c>
       <c r="C5" t="b">
         <v>0</v>
@@ -2419,10 +2419,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75">
       <c r="A6" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>78</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>79</v>
       </c>
       <c r="C6" t="b">
         <v>0</v>
@@ -2430,10 +2430,10 @@
     </row>
     <row r="7" spans="1:3" ht="15.75">
       <c r="A7" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>80</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>81</v>
       </c>
       <c r="C7" t="b">
         <v>0</v>
@@ -2441,10 +2441,10 @@
     </row>
     <row r="8" spans="1:3" ht="15.75">
       <c r="A8" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>82</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>83</v>
       </c>
       <c r="C8" t="b">
         <v>0</v>
@@ -2452,10 +2452,10 @@
     </row>
     <row r="9" spans="1:3" ht="15.75">
       <c r="A9" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>84</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>85</v>
       </c>
       <c r="C9" t="b">
         <v>0</v>
@@ -2463,10 +2463,10 @@
     </row>
     <row r="10" spans="1:3" ht="15.75">
       <c r="A10" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>86</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>87</v>
       </c>
       <c r="C10" t="b">
         <v>0</v>
@@ -2474,10 +2474,10 @@
     </row>
     <row r="11" spans="1:3" ht="15.75">
       <c r="A11" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>88</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>89</v>
       </c>
       <c r="C11" t="b">
         <v>0</v>
@@ -2485,10 +2485,10 @@
     </row>
     <row r="12" spans="1:3" ht="15.75">
       <c r="A12" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>90</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>91</v>
       </c>
       <c r="C12" t="b">
         <v>0</v>
@@ -2496,10 +2496,10 @@
     </row>
     <row r="13" spans="1:3" ht="15.75">
       <c r="A13" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B13" s="8" t="s">
         <v>92</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>93</v>
       </c>
       <c r="C13" t="b">
         <v>0</v>
@@ -2507,10 +2507,10 @@
     </row>
     <row r="14" spans="1:3" ht="15.75">
       <c r="A14" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B14" s="8" t="s">
         <v>94</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>95</v>
       </c>
       <c r="C14" t="b">
         <v>0</v>
@@ -2518,10 +2518,10 @@
     </row>
     <row r="15" spans="1:3" ht="15.75">
       <c r="A15" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B15" s="8" t="s">
         <v>96</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>97</v>
       </c>
       <c r="C15" t="b">
         <v>0</v>
@@ -2529,10 +2529,10 @@
     </row>
     <row r="16" spans="1:3" ht="15.75">
       <c r="A16" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="C16" t="b">
         <v>0</v>
@@ -2540,10 +2540,10 @@
     </row>
     <row r="17" spans="1:3" ht="15.75">
       <c r="A17" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>100</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>101</v>
       </c>
       <c r="C17" t="b">
         <v>0</v>
@@ -2551,10 +2551,10 @@
     </row>
     <row r="18" spans="1:3" ht="15.75">
       <c r="A18" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B18" s="8" t="s">
         <v>102</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>103</v>
       </c>
       <c r="C18" t="b">
         <v>0</v>
@@ -2562,10 +2562,10 @@
     </row>
     <row r="19" spans="1:3" ht="15.75">
       <c r="A19" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="B19" s="8" t="s">
         <v>104</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>105</v>
       </c>
       <c r="C19" t="b">
         <v>0</v>
@@ -2573,10 +2573,10 @@
     </row>
     <row r="20" spans="1:3" ht="15.75">
       <c r="A20" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B20" s="8" t="s">
         <v>106</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>107</v>
       </c>
       <c r="C20" t="b">
         <v>0</v>
@@ -2584,10 +2584,10 @@
     </row>
     <row r="21" spans="1:3" ht="15.75">
       <c r="A21" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B21" s="8" t="s">
         <v>108</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>109</v>
       </c>
       <c r="C21" t="b">
         <v>0</v>
@@ -2595,10 +2595,10 @@
     </row>
     <row r="22" spans="1:3" ht="15.75">
       <c r="A22" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B22" s="8" t="s">
         <v>110</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>111</v>
       </c>
       <c r="C22" t="b">
         <v>0</v>
@@ -2606,10 +2606,10 @@
     </row>
     <row r="23" spans="1:3" ht="15.75">
       <c r="A23" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B23" s="8" t="s">
         <v>112</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>113</v>
       </c>
       <c r="C23" t="b">
         <v>0</v>
@@ -2617,10 +2617,10 @@
     </row>
     <row r="24" spans="1:3" ht="15.75">
       <c r="A24" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B24" s="8" t="s">
         <v>114</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>115</v>
       </c>
       <c r="C24" t="b">
         <v>0</v>
@@ -2628,10 +2628,10 @@
     </row>
     <row r="25" spans="1:3" ht="15.75">
       <c r="A25" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B25" s="8" t="s">
         <v>116</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>117</v>
       </c>
       <c r="C25" t="b">
         <v>0</v>
@@ -2639,10 +2639,10 @@
     </row>
     <row r="26" spans="1:3" ht="15.75">
       <c r="A26" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B26" s="8" t="s">
         <v>118</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>119</v>
       </c>
       <c r="C26" t="b">
         <v>0</v>
@@ -2650,10 +2650,10 @@
     </row>
     <row r="27" spans="1:3" ht="15.75">
       <c r="A27" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B27" s="8" t="s">
         <v>120</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>121</v>
       </c>
       <c r="C27" t="b">
         <v>0</v>
@@ -2661,10 +2661,10 @@
     </row>
     <row r="28" spans="1:3" ht="15.75">
       <c r="A28" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B28" s="8" t="s">
         <v>122</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>123</v>
       </c>
       <c r="C28" t="b">
         <v>0</v>
@@ -2672,10 +2672,10 @@
     </row>
     <row r="29" spans="1:3" ht="15.75">
       <c r="A29" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B29" s="8" t="s">
         <v>124</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>125</v>
       </c>
       <c r="C29" t="b">
         <v>0</v>
@@ -2683,10 +2683,10 @@
     </row>
     <row r="30" spans="1:3" ht="15.75">
       <c r="A30" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="B30" s="8" t="s">
         <v>126</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>127</v>
       </c>
       <c r="C30" t="b">
         <v>0</v>
@@ -2694,10 +2694,10 @@
     </row>
     <row r="31" spans="1:3" ht="15.75">
       <c r="A31" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B31" s="8" t="s">
         <v>128</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>129</v>
       </c>
       <c r="C31" t="b">
         <v>0</v>
@@ -2705,10 +2705,10 @@
     </row>
     <row r="32" spans="1:3" ht="15.75">
       <c r="A32" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B32" s="8" t="s">
         <v>130</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>131</v>
       </c>
       <c r="C32" t="b">
         <v>0</v>
@@ -2716,10 +2716,10 @@
     </row>
     <row r="33" spans="1:3" ht="15.75">
       <c r="A33" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="B33" s="8" t="s">
         <v>132</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>133</v>
       </c>
       <c r="C33" t="b">
         <v>0</v>
@@ -2727,10 +2727,10 @@
     </row>
     <row r="34" spans="1:3" ht="15.75">
       <c r="A34" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B34" s="8" t="s">
         <v>134</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>135</v>
       </c>
       <c r="C34" t="b">
         <v>0</v>
@@ -2738,10 +2738,10 @@
     </row>
     <row r="35" spans="1:3" ht="15.75">
       <c r="A35" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="B35" s="8" t="s">
         <v>136</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>137</v>
       </c>
       <c r="C35" t="b">
         <v>0</v>
@@ -2749,10 +2749,10 @@
     </row>
     <row r="36" spans="1:3" ht="15.75">
       <c r="A36" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="B36" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>139</v>
       </c>
       <c r="C36" t="b">
         <v>0</v>
@@ -2760,10 +2760,10 @@
     </row>
     <row r="37" spans="1:3" ht="15.75">
       <c r="A37" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B37" s="8" t="s">
         <v>140</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>141</v>
       </c>
       <c r="C37" t="b">
         <v>0</v>
@@ -2771,10 +2771,10 @@
     </row>
     <row r="38" spans="1:3" ht="15.75">
       <c r="A38" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="B38" s="8" t="s">
         <v>142</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>143</v>
       </c>
       <c r="C38" t="b">
         <v>0</v>
@@ -2782,10 +2782,10 @@
     </row>
     <row r="39" spans="1:3" ht="15.75">
       <c r="A39" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="B39" s="8" t="s">
         <v>144</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>145</v>
       </c>
       <c r="C39" t="b">
         <v>0</v>
@@ -2793,10 +2793,10 @@
     </row>
     <row r="40" spans="1:3" ht="15.75">
       <c r="A40" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="B40" s="8" t="s">
         <v>146</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>147</v>
       </c>
       <c r="C40" t="b">
         <v>0</v>
@@ -2804,10 +2804,10 @@
     </row>
     <row r="41" spans="1:3" ht="15.75">
       <c r="A41" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="B41" s="8" t="s">
         <v>148</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>149</v>
       </c>
       <c r="C41" t="b">
         <v>0</v>
@@ -2815,10 +2815,10 @@
     </row>
     <row r="42" spans="1:3" ht="15.75">
       <c r="A42" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="B42" s="8" t="s">
         <v>150</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>151</v>
       </c>
       <c r="C42" t="b">
         <v>0</v>
@@ -2826,10 +2826,10 @@
     </row>
     <row r="43" spans="1:3" ht="15.75">
       <c r="A43" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B43" s="8" t="s">
         <v>152</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>153</v>
       </c>
       <c r="C43" t="b">
         <v>0</v>
@@ -2837,10 +2837,10 @@
     </row>
     <row r="44" spans="1:3" ht="15.75">
       <c r="A44" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="B44" s="8" t="s">
         <v>154</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>155</v>
       </c>
       <c r="C44" t="b">
         <v>0</v>
@@ -2848,10 +2848,10 @@
     </row>
     <row r="45" spans="1:3" ht="15.75">
       <c r="A45" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B45" s="8" t="s">
         <v>156</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>157</v>
       </c>
       <c r="C45" t="b">
         <v>0</v>
@@ -2859,10 +2859,10 @@
     </row>
     <row r="46" spans="1:3" ht="15.75">
       <c r="A46" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="B46" s="8" t="s">
         <v>158</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>159</v>
       </c>
       <c r="C46" t="b">
         <v>0</v>
@@ -2870,10 +2870,10 @@
     </row>
     <row r="47" spans="1:3" ht="15.75">
       <c r="A47" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="B47" s="8" t="s">
         <v>160</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>161</v>
       </c>
       <c r="C47" t="b">
         <v>0</v>
@@ -2881,10 +2881,10 @@
     </row>
     <row r="48" spans="1:3" ht="15.75">
       <c r="A48" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="B48" s="8" t="s">
         <v>162</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>163</v>
       </c>
       <c r="C48" t="b">
         <v>0</v>
@@ -2892,10 +2892,10 @@
     </row>
     <row r="49" spans="1:3" ht="15.75">
       <c r="A49" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B49" s="8" t="s">
         <v>164</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>165</v>
       </c>
       <c r="C49" t="b">
         <v>0</v>
@@ -2903,10 +2903,10 @@
     </row>
     <row r="50" spans="1:3" ht="15.75">
       <c r="A50" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="B50" s="8" t="s">
         <v>166</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>167</v>
       </c>
       <c r="C50" t="b">
         <v>0</v>
@@ -2914,10 +2914,10 @@
     </row>
     <row r="51" spans="1:3" ht="15.75">
       <c r="A51" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="B51" s="8" t="s">
         <v>168</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>169</v>
       </c>
       <c r="C51" t="b">
         <v>0</v>
@@ -2925,10 +2925,10 @@
     </row>
     <row r="52" spans="1:3" ht="15.75">
       <c r="A52" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B52" s="8" t="s">
         <v>170</v>
-      </c>
-      <c r="B52" s="8" t="s">
-        <v>171</v>
       </c>
       <c r="C52" t="b">
         <v>0</v>
@@ -2936,10 +2936,10 @@
     </row>
     <row r="53" spans="1:3" ht="15.75">
       <c r="A53" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="B53" s="8" t="s">
         <v>172</v>
-      </c>
-      <c r="B53" s="8" t="s">
-        <v>173</v>
       </c>
       <c r="C53" t="b">
         <v>0</v>
@@ -2947,10 +2947,10 @@
     </row>
     <row r="54" spans="1:3" ht="15.75">
       <c r="A54" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="B54" s="8" t="s">
         <v>174</v>
-      </c>
-      <c r="B54" s="8" t="s">
-        <v>175</v>
       </c>
       <c r="C54" t="b">
         <v>0</v>
@@ -2958,10 +2958,10 @@
     </row>
     <row r="55" spans="1:3" ht="15.75">
       <c r="A55" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="B55" s="8" t="s">
         <v>176</v>
-      </c>
-      <c r="B55" s="8" t="s">
-        <v>177</v>
       </c>
       <c r="C55" t="b">
         <v>0</v>
@@ -2969,10 +2969,10 @@
     </row>
     <row r="56" spans="1:3" ht="15.75">
       <c r="A56" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="B56" s="8" t="s">
         <v>178</v>
-      </c>
-      <c r="B56" s="8" t="s">
-        <v>179</v>
       </c>
       <c r="C56" t="b">
         <v>0</v>
@@ -2980,10 +2980,10 @@
     </row>
     <row r="57" spans="1:3" ht="15.75">
       <c r="A57" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="B57" s="8" t="s">
         <v>180</v>
-      </c>
-      <c r="B57" s="8" t="s">
-        <v>181</v>
       </c>
       <c r="C57" t="b">
         <v>0</v>
@@ -2991,10 +2991,10 @@
     </row>
     <row r="58" spans="1:3" ht="15.75">
       <c r="A58" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="B58" s="8" t="s">
         <v>182</v>
-      </c>
-      <c r="B58" s="8" t="s">
-        <v>183</v>
       </c>
       <c r="C58" t="b">
         <v>0</v>
@@ -3002,10 +3002,10 @@
     </row>
     <row r="59" spans="1:3" ht="15.75">
       <c r="A59" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B59" s="8" t="s">
         <v>184</v>
-      </c>
-      <c r="B59" s="8" t="s">
-        <v>185</v>
       </c>
       <c r="C59" t="b">
         <v>0</v>
@@ -3013,10 +3013,10 @@
     </row>
     <row r="60" spans="1:3" ht="15.75">
       <c r="A60" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="B60" s="8" t="s">
         <v>186</v>
-      </c>
-      <c r="B60" s="8" t="s">
-        <v>187</v>
       </c>
       <c r="C60" t="b">
         <v>0</v>
@@ -3024,10 +3024,10 @@
     </row>
     <row r="61" spans="1:3" ht="15.75">
       <c r="A61" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="B61" s="8" t="s">
         <v>188</v>
-      </c>
-      <c r="B61" s="8" t="s">
-        <v>189</v>
       </c>
       <c r="C61" t="b">
         <v>0</v>
@@ -3035,10 +3035,10 @@
     </row>
     <row r="62" spans="1:3" ht="15.75">
       <c r="A62" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="B62" s="8" t="s">
         <v>190</v>
-      </c>
-      <c r="B62" s="8" t="s">
-        <v>191</v>
       </c>
       <c r="C62" t="b">
         <v>0</v>
@@ -3046,10 +3046,10 @@
     </row>
     <row r="63" spans="1:3" ht="15.75">
       <c r="A63" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="B63" s="8" t="s">
         <v>192</v>
-      </c>
-      <c r="B63" s="8" t="s">
-        <v>193</v>
       </c>
       <c r="C63" t="b">
         <v>0</v>
@@ -3057,10 +3057,10 @@
     </row>
     <row r="64" spans="1:3" ht="15.75">
       <c r="A64" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="B64" s="8" t="s">
         <v>194</v>
-      </c>
-      <c r="B64" s="8" t="s">
-        <v>195</v>
       </c>
       <c r="C64" t="b">
         <v>0</v>
@@ -3068,10 +3068,10 @@
     </row>
     <row r="65" spans="1:3" ht="15.75">
       <c r="A65" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C65" t="b">
         <v>1</v>
@@ -3079,10 +3079,10 @@
     </row>
     <row r="66" spans="1:3" ht="15.75">
       <c r="A66" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C66" t="b">
         <v>1</v>
@@ -3090,10 +3090,10 @@
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B67" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C67" t="b">
         <v>1</v>
@@ -3101,10 +3101,10 @@
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B68" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C68" t="b">
         <v>1</v>
@@ -3112,10 +3112,10 @@
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B69" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C69" t="b">
         <v>1</v>
@@ -3123,10 +3123,10 @@
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B70" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C70" t="b">
         <v>1</v>
@@ -3134,10 +3134,10 @@
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B71" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C71" t="b">
         <v>1</v>
@@ -3145,10 +3145,10 @@
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B72" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C72" t="b">
         <v>1</v>
@@ -3156,10 +3156,10 @@
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B73" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C73" t="b">
         <v>1</v>
@@ -3167,10 +3167,10 @@
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B74" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C74" t="b">
         <v>1</v>
@@ -3178,10 +3178,10 @@
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B75" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C75" t="b">
         <v>1</v>
@@ -3189,10 +3189,10 @@
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B76" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C76" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Tweaking database queries for watchlist
</commit_message>
<xml_diff>
--- a/resources/test_data_user.xlsx
+++ b/resources/test_data_user.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\OneDrive - UNSW\University\Postgraduate\Year 3 Trimester 3\COMP9900\Project\BackEnd\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC440469-20AE-475B-BC88-DE6A5C774361}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD69D1AE-BC2B-470C-9F29-1C54884FC7F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14610" windowHeight="21000" xr2:uid="{1A28855D-1372-4992-8C97-28705A0C69E1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13155" windowHeight="21000" activeTab="6" xr2:uid="{1A28855D-1372-4992-8C97-28705A0C69E1}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="210">
   <si>
     <t>j.meraachli@student.unsw.edu.au</t>
   </si>
@@ -679,12 +679,15 @@
   <si>
     <t>quote</t>
   </si>
+  <si>
+    <t>priority</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -729,6 +732,11 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -751,7 +759,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -767,6 +775,7 @@
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1105,7 +1114,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36BB9172-4BA3-48EB-851A-CC045B92290E}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -2356,18 +2365,19 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB0AE7CC-0281-42AB-BEFB-FF7CDAA66D40}">
-  <dimension ref="A1:C76"/>
+  <dimension ref="A1:D76"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="B79" sqref="B79"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="70" customWidth="1"/>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75">
+    <row r="1" spans="1:4" ht="15.75">
       <c r="A1" s="8" t="s">
         <v>68</v>
       </c>
@@ -2377,8 +2387,11 @@
       <c r="C1" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75">
+      <c r="D1" s="9" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75">
       <c r="A2" s="8" t="s">
         <v>69</v>
       </c>
@@ -2389,7 +2402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75">
+    <row r="3" spans="1:4" ht="15.75">
       <c r="A3" s="8" t="s">
         <v>71</v>
       </c>
@@ -2400,7 +2413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75">
+    <row r="4" spans="1:4" ht="15.75">
       <c r="A4" s="8" t="s">
         <v>73</v>
       </c>
@@ -2410,8 +2423,11 @@
       <c r="C4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.75">
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75">
       <c r="A5" s="8" t="s">
         <v>75</v>
       </c>
@@ -2422,7 +2438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75">
+    <row r="6" spans="1:4" ht="15.75">
       <c r="A6" s="8" t="s">
         <v>77</v>
       </c>
@@ -2433,7 +2449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75">
+    <row r="7" spans="1:4" ht="15.75">
       <c r="A7" s="8" t="s">
         <v>79</v>
       </c>
@@ -2444,7 +2460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75">
+    <row r="8" spans="1:4" ht="15.75">
       <c r="A8" s="8" t="s">
         <v>81</v>
       </c>
@@ -2455,7 +2471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75">
+    <row r="9" spans="1:4" ht="15.75">
       <c r="A9" s="8" t="s">
         <v>83</v>
       </c>
@@ -2466,7 +2482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75">
+    <row r="10" spans="1:4" ht="15.75">
       <c r="A10" s="8" t="s">
         <v>85</v>
       </c>
@@ -2477,7 +2493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75">
+    <row r="11" spans="1:4" ht="15.75">
       <c r="A11" s="8" t="s">
         <v>87</v>
       </c>
@@ -2488,7 +2504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75">
+    <row r="12" spans="1:4" ht="15.75">
       <c r="A12" s="8" t="s">
         <v>89</v>
       </c>
@@ -2498,8 +2514,11 @@
       <c r="C12" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="15.75">
+      <c r="D12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.75">
       <c r="A13" s="8" t="s">
         <v>91</v>
       </c>
@@ -2509,8 +2528,11 @@
       <c r="C13" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="15.75">
+      <c r="D13">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.75">
       <c r="A14" s="8" t="s">
         <v>93</v>
       </c>
@@ -2521,7 +2543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.75">
+    <row r="15" spans="1:4" ht="15.75">
       <c r="A15" s="8" t="s">
         <v>95</v>
       </c>
@@ -2531,8 +2553,11 @@
       <c r="C15" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="15.75">
+      <c r="D15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.75">
       <c r="A16" s="8" t="s">
         <v>97</v>
       </c>
@@ -2543,7 +2568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.75">
+    <row r="17" spans="1:4" ht="15.75">
       <c r="A17" s="8" t="s">
         <v>99</v>
       </c>
@@ -2554,7 +2579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75">
+    <row r="18" spans="1:4" ht="15.75">
       <c r="A18" s="8" t="s">
         <v>101</v>
       </c>
@@ -2564,8 +2589,11 @@
       <c r="C18" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="15.75">
+      <c r="D18">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75">
       <c r="A19" s="8" t="s">
         <v>103</v>
       </c>
@@ -2575,8 +2603,11 @@
       <c r="C19" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="15.75">
+      <c r="D19">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75">
       <c r="A20" s="8" t="s">
         <v>105</v>
       </c>
@@ -2586,8 +2617,11 @@
       <c r="C20" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="15.75">
+      <c r="D20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75">
       <c r="A21" s="8" t="s">
         <v>107</v>
       </c>
@@ -2598,7 +2632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.75">
+    <row r="22" spans="1:4" ht="15.75">
       <c r="A22" s="8" t="s">
         <v>109</v>
       </c>
@@ -2608,8 +2642,11 @@
       <c r="C22" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="15.75">
+      <c r="D22">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.75">
       <c r="A23" s="8" t="s">
         <v>111</v>
       </c>
@@ -2620,7 +2657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15.75">
+    <row r="24" spans="1:4" ht="15.75">
       <c r="A24" s="8" t="s">
         <v>113</v>
       </c>
@@ -2631,7 +2668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.75">
+    <row r="25" spans="1:4" ht="15.75">
       <c r="A25" s="8" t="s">
         <v>115</v>
       </c>
@@ -2642,7 +2679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15.75">
+    <row r="26" spans="1:4" ht="15.75">
       <c r="A26" s="8" t="s">
         <v>117</v>
       </c>
@@ -2653,7 +2690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15.75">
+    <row r="27" spans="1:4" ht="15.75">
       <c r="A27" s="8" t="s">
         <v>119</v>
       </c>
@@ -2664,7 +2701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75">
+    <row r="28" spans="1:4" ht="15.75">
       <c r="A28" s="8" t="s">
         <v>121</v>
       </c>
@@ -2674,8 +2711,11 @@
       <c r="C28" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="15.75">
+      <c r="D28">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15.75">
       <c r="A29" s="8" t="s">
         <v>123</v>
       </c>
@@ -2685,8 +2725,11 @@
       <c r="C29" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="15.75">
+      <c r="D29">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15.75">
       <c r="A30" s="8" t="s">
         <v>125</v>
       </c>
@@ -2696,8 +2739,11 @@
       <c r="C30" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="15.75">
+      <c r="D30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15.75">
       <c r="A31" s="8" t="s">
         <v>127</v>
       </c>
@@ -2708,7 +2754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15.75">
+    <row r="32" spans="1:4" ht="15.75">
       <c r="A32" s="8" t="s">
         <v>129</v>
       </c>
@@ -2719,7 +2765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.75">
+    <row r="33" spans="1:4" ht="15.75">
       <c r="A33" s="8" t="s">
         <v>131</v>
       </c>
@@ -2730,7 +2776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15.75">
+    <row r="34" spans="1:4" ht="15.75">
       <c r="A34" s="8" t="s">
         <v>133</v>
       </c>
@@ -2741,7 +2787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="15.75">
+    <row r="35" spans="1:4" ht="15.75">
       <c r="A35" s="8" t="s">
         <v>135</v>
       </c>
@@ -2752,7 +2798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15.75">
+    <row r="36" spans="1:4" ht="15.75">
       <c r="A36" s="8" t="s">
         <v>137</v>
       </c>
@@ -2763,7 +2809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15.75">
+    <row r="37" spans="1:4" ht="15.75">
       <c r="A37" s="8" t="s">
         <v>139</v>
       </c>
@@ -2774,7 +2820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="15.75">
+    <row r="38" spans="1:4" ht="15.75">
       <c r="A38" s="8" t="s">
         <v>141</v>
       </c>
@@ -2785,7 +2831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="15.75">
+    <row r="39" spans="1:4" ht="15.75">
       <c r="A39" s="8" t="s">
         <v>143</v>
       </c>
@@ -2795,8 +2841,11 @@
       <c r="C39" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" ht="15.75">
+      <c r="D39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15.75">
       <c r="A40" s="8" t="s">
         <v>145</v>
       </c>
@@ -2807,7 +2856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="15.75">
+    <row r="41" spans="1:4" ht="15.75">
       <c r="A41" s="8" t="s">
         <v>147</v>
       </c>
@@ -2818,7 +2867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15.75">
+    <row r="42" spans="1:4" ht="15.75">
       <c r="A42" s="8" t="s">
         <v>149</v>
       </c>
@@ -2828,8 +2877,11 @@
       <c r="C42" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" ht="15.75">
+      <c r="D42">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="15.75">
       <c r="A43" s="8" t="s">
         <v>151</v>
       </c>
@@ -2840,7 +2892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="15.75">
+    <row r="44" spans="1:4" ht="15.75">
       <c r="A44" s="8" t="s">
         <v>153</v>
       </c>
@@ -2851,7 +2903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="15.75">
+    <row r="45" spans="1:4" ht="15.75">
       <c r="A45" s="8" t="s">
         <v>155</v>
       </c>
@@ -2862,7 +2914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="15.75">
+    <row r="46" spans="1:4" ht="15.75">
       <c r="A46" s="8" t="s">
         <v>157</v>
       </c>
@@ -2873,7 +2925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="15.75">
+    <row r="47" spans="1:4" ht="15.75">
       <c r="A47" s="8" t="s">
         <v>159</v>
       </c>
@@ -2884,7 +2936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="15.75">
+    <row r="48" spans="1:4" ht="15.75">
       <c r="A48" s="8" t="s">
         <v>161</v>
       </c>
@@ -2895,7 +2947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="15.75">
+    <row r="49" spans="1:4" ht="15.75">
       <c r="A49" s="8" t="s">
         <v>163</v>
       </c>
@@ -2906,7 +2958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="15.75">
+    <row r="50" spans="1:4" ht="15.75">
       <c r="A50" s="8" t="s">
         <v>165</v>
       </c>
@@ -2917,7 +2969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="15.75">
+    <row r="51" spans="1:4" ht="15.75">
       <c r="A51" s="8" t="s">
         <v>167</v>
       </c>
@@ -2927,8 +2979,11 @@
       <c r="C51" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" ht="15.75">
+      <c r="D51">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="15.75">
       <c r="A52" s="8" t="s">
         <v>169</v>
       </c>
@@ -2938,8 +2993,11 @@
       <c r="C52" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" ht="15.75">
+      <c r="D52">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="15.75">
       <c r="A53" s="8" t="s">
         <v>171</v>
       </c>
@@ -2949,8 +3007,11 @@
       <c r="C53" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" ht="15.75">
+      <c r="D53">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="15.75">
       <c r="A54" s="8" t="s">
         <v>173</v>
       </c>
@@ -2960,8 +3021,11 @@
       <c r="C54" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" ht="15.75">
+      <c r="D54">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="15.75">
       <c r="A55" s="8" t="s">
         <v>175</v>
       </c>
@@ -2972,7 +3036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="15.75">
+    <row r="56" spans="1:4" ht="15.75">
       <c r="A56" s="8" t="s">
         <v>177</v>
       </c>
@@ -2983,7 +3047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="15.75">
+    <row r="57" spans="1:4" ht="15.75">
       <c r="A57" s="8" t="s">
         <v>179</v>
       </c>
@@ -2993,8 +3057,11 @@
       <c r="C57" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" ht="15.75">
+      <c r="D57">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="15.75">
       <c r="A58" s="8" t="s">
         <v>181</v>
       </c>
@@ -3005,7 +3072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="15.75">
+    <row r="59" spans="1:4" ht="15.75">
       <c r="A59" s="8" t="s">
         <v>183</v>
       </c>
@@ -3015,8 +3082,11 @@
       <c r="C59" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" ht="15.75">
+      <c r="D59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="15.75">
       <c r="A60" s="8" t="s">
         <v>185</v>
       </c>
@@ -3027,7 +3097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="15.75">
+    <row r="61" spans="1:4" ht="15.75">
       <c r="A61" s="8" t="s">
         <v>187</v>
       </c>
@@ -3037,8 +3107,11 @@
       <c r="C61" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" ht="15.75">
+      <c r="D61">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="15.75">
       <c r="A62" s="8" t="s">
         <v>189</v>
       </c>
@@ -3049,7 +3122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="15.75">
+    <row r="63" spans="1:4" ht="15.75">
       <c r="A63" s="8" t="s">
         <v>191</v>
       </c>
@@ -3060,7 +3133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="15.75">
+    <row r="64" spans="1:4" ht="15.75">
       <c r="A64" s="8" t="s">
         <v>193</v>
       </c>
@@ -3070,8 +3143,11 @@
       <c r="C64" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" ht="15.75">
+      <c r="D64">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="15.75">
       <c r="A65" s="8" t="s">
         <v>196</v>
       </c>
@@ -3081,8 +3157,11 @@
       <c r="C65" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" ht="15.75">
+      <c r="D65">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="15.75">
       <c r="A66" s="8" t="s">
         <v>197</v>
       </c>
@@ -3092,8 +3171,11 @@
       <c r="C66" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="1:3">
+      <c r="D66">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
       <c r="A67" t="s">
         <v>198</v>
       </c>
@@ -3103,8 +3185,11 @@
       <c r="C67" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="68" spans="1:3">
+      <c r="D67">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
       <c r="A68" t="s">
         <v>199</v>
       </c>
@@ -3114,8 +3199,11 @@
       <c r="C68" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="69" spans="1:3">
+      <c r="D68">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
       <c r="A69" t="s">
         <v>200</v>
       </c>
@@ -3125,8 +3213,11 @@
       <c r="C69" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="1:3">
+      <c r="D69">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
       <c r="A70" t="s">
         <v>201</v>
       </c>
@@ -3136,8 +3227,11 @@
       <c r="C70" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:3">
+      <c r="D70">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
       <c r="A71" t="s">
         <v>202</v>
       </c>
@@ -3147,8 +3241,11 @@
       <c r="C71" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="1:3">
+      <c r="D71">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
       <c r="A72" t="s">
         <v>203</v>
       </c>
@@ -3158,8 +3255,11 @@
       <c r="C72" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="73" spans="1:3">
+      <c r="D72">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
       <c r="A73" t="s">
         <v>204</v>
       </c>
@@ -3169,8 +3269,11 @@
       <c r="C73" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:3">
+      <c r="D73">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
       <c r="A74" t="s">
         <v>205</v>
       </c>
@@ -3180,8 +3283,11 @@
       <c r="C74" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:3">
+      <c r="D74">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
       <c r="A75" t="s">
         <v>206</v>
       </c>
@@ -3191,8 +3297,11 @@
       <c r="C75" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:3">
+      <c r="D75">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
       <c r="A76" t="s">
         <v>207</v>
       </c>
@@ -3201,6 +3310,9 @@
       </c>
       <c r="C76" t="b">
         <v>1</v>
+      </c>
+      <c r="D76">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixing database relationships and insertion
</commit_message>
<xml_diff>
--- a/resources/test_data_user.xlsx
+++ b/resources/test_data_user.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unsw-my.sharepoint.com/personal/z5020362_ad_unsw_edu_au/Documents/University/Postgraduate/Year 3 Trimester 3/COMP9900/Project/BackEnd/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{A297C295-65EC-4B41-8727-F90BF0EBFD20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6E982700-168C-4E6A-82A4-F58449C2381F}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{A297C295-65EC-4B41-8727-F90BF0EBFD20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{14CF9051-B0D8-4B5C-9D95-9D8F4321267B}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="25800" windowHeight="21000" activeTab="1" xr2:uid="{1A28855D-1372-4992-8C97-28705A0C69E1}"/>
+    <workbookView xWindow="390" yWindow="0" windowWidth="25800" windowHeight="21000" activeTab="5" xr2:uid="{1A28855D-1372-4992-8C97-28705A0C69E1}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="212">
   <si>
     <t>j.meraachli@student.unsw.edu.au</t>
   </si>
@@ -212,12 +212,6 @@
     <t>Microsoft</t>
   </si>
   <si>
-    <t>Pricewaterhouse Cooper</t>
-  </si>
-  <si>
-    <t>KPMG Ltd</t>
-  </si>
-  <si>
     <t>transaction</t>
   </si>
   <si>
@@ -690,6 +684,18 @@
   </si>
   <si>
     <t>AAPL</t>
+  </si>
+  <si>
+    <t>ZIP</t>
+  </si>
+  <si>
+    <t>Zip</t>
+  </si>
+  <si>
+    <t>TSLA</t>
+  </si>
+  <si>
+    <t>Tesla Inc.</t>
   </si>
 </sst>
 </file>
@@ -1167,10 +1173,10 @@
         <v>23</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -1178,7 +1184,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -1200,7 +1206,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -1222,7 +1228,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
@@ -1244,7 +1250,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -1266,7 +1272,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C6" t="s">
         <v>14</v>
@@ -1297,7 +1303,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF8D5324-5018-9640-9915-418B2F181888}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
@@ -1316,7 +1322,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1457,7 +1463,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:F7"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -1564,10 +1570,10 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>208</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>209</v>
       </c>
       <c r="C6" t="s">
         <v>36</v>
@@ -1584,10 +1590,10 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>210</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>211</v>
       </c>
       <c r="C7" t="s">
         <v>36</v>
@@ -1612,7 +1618,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1630,10 +1636,10 @@
         <v>41</v>
       </c>
       <c r="C1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1641,7 +1647,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1649,7 +1655,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1657,7 +1663,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1665,7 +1671,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1673,7 +1679,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1686,7 +1692,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B6"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1790,12 +1796,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{839B1F08-9FB4-4205-9D29-58AB9BDB11FE}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" customWidth="1"/>
     <col min="6" max="6" width="26.42578125" customWidth="1"/>
   </cols>
@@ -1811,19 +1818,19 @@
         <v>27</v>
       </c>
       <c r="D1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F1" t="s">
         <v>43</v>
       </c>
       <c r="G1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1834,13 +1841,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>207</v>
       </c>
       <c r="D2">
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F2" s="6">
         <v>44119.108414351853</v>
@@ -1866,7 +1873,7 @@
         <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F3" s="6">
         <v>44119.108414351853</v>
@@ -1892,7 +1899,7 @@
         <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F4" s="5">
         <v>44119.108419884258</v>
@@ -1912,13 +1919,13 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>98</v>
       </c>
       <c r="D5">
         <v>40</v>
       </c>
       <c r="E5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F5" s="5">
         <v>44119.108419884258</v>
@@ -1938,13 +1945,13 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>210</v>
       </c>
       <c r="D6">
         <v>50</v>
       </c>
       <c r="E6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F6" s="5">
         <v>44119.108419884258</v>
@@ -1970,7 +1977,7 @@
         <v>60</v>
       </c>
       <c r="E7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F7" s="6">
         <v>44119.108414351853</v>
@@ -1990,13 +1997,13 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>207</v>
       </c>
       <c r="D8">
         <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F8" s="6">
         <v>44119.233414351853</v>
@@ -2022,7 +2029,7 @@
         <v>20</v>
       </c>
       <c r="E9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F9" s="6">
         <v>44119.275081018517</v>
@@ -2042,13 +2049,13 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>207</v>
       </c>
       <c r="D10">
         <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F10" s="6">
         <v>44119.441747685189</v>
@@ -2074,7 +2081,7 @@
         <v>20</v>
       </c>
       <c r="E11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F11" s="6">
         <v>44119.441747685189</v>
@@ -2100,7 +2107,7 @@
         <v>30</v>
       </c>
       <c r="E12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F12" s="6">
         <v>44119.441747685189</v>
@@ -2120,13 +2127,13 @@
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>47</v>
+        <v>98</v>
       </c>
       <c r="D13">
         <v>40</v>
       </c>
       <c r="E13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F13" s="6">
         <v>44119.441747685189</v>
@@ -2152,7 +2159,7 @@
         <v>30</v>
       </c>
       <c r="E14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F14" s="6">
         <v>44119.441747685189</v>
@@ -2172,13 +2179,13 @@
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>47</v>
+        <v>98</v>
       </c>
       <c r="D15">
         <v>40</v>
       </c>
       <c r="E15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F15" s="6">
         <v>44119.441747685189</v>
@@ -2198,13 +2205,13 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
+        <v>207</v>
       </c>
       <c r="D16">
         <v>10</v>
       </c>
       <c r="E16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F16" s="6">
         <v>44119.441747685189</v>
@@ -2224,13 +2231,13 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>45</v>
+        <v>207</v>
       </c>
       <c r="D17">
         <v>20</v>
       </c>
       <c r="E17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F17" s="6">
         <v>44119.441747685189</v>
@@ -2256,7 +2263,7 @@
         <v>60</v>
       </c>
       <c r="E18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F18" s="6">
         <v>44119.483414351853</v>
@@ -2276,13 +2283,13 @@
         <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>46</v>
+        <v>210</v>
       </c>
       <c r="D19">
         <v>60</v>
       </c>
       <c r="E19" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F19" s="6">
         <v>44119.483414351853</v>
@@ -2308,7 +2315,7 @@
         <v>60</v>
       </c>
       <c r="E20" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F20" s="6">
         <v>44119.483414351853</v>
@@ -2328,13 +2335,13 @@
         <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>46</v>
+        <v>210</v>
       </c>
       <c r="D21">
         <v>60</v>
       </c>
       <c r="E21" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F21" s="6">
         <v>44119.483414351853</v>
@@ -2380,24 +2387,24 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75">
       <c r="A1" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75">
       <c r="A2" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C2" t="b">
         <v>0</v>
@@ -2405,10 +2412,10 @@
     </row>
     <row r="3" spans="1:4" ht="15.75">
       <c r="A3" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
@@ -2416,10 +2423,10 @@
     </row>
     <row r="4" spans="1:4" ht="15.75">
       <c r="A4" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C4" t="b">
         <v>0</v>
@@ -2427,10 +2434,10 @@
     </row>
     <row r="5" spans="1:4" ht="15.75">
       <c r="A5" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C5" t="b">
         <v>0</v>
@@ -2438,10 +2445,10 @@
     </row>
     <row r="6" spans="1:4" ht="15.75">
       <c r="A6" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C6" t="b">
         <v>0</v>
@@ -2449,10 +2456,10 @@
     </row>
     <row r="7" spans="1:4" ht="15.75">
       <c r="A7" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C7" t="b">
         <v>0</v>
@@ -2460,10 +2467,10 @@
     </row>
     <row r="8" spans="1:4" ht="15.75">
       <c r="A8" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C8" t="b">
         <v>0</v>
@@ -2471,10 +2478,10 @@
     </row>
     <row r="9" spans="1:4" ht="15.75">
       <c r="A9" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C9" t="b">
         <v>0</v>
@@ -2482,10 +2489,10 @@
     </row>
     <row r="10" spans="1:4" ht="15.75">
       <c r="A10" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C10" t="b">
         <v>0</v>
@@ -2493,10 +2500,10 @@
     </row>
     <row r="11" spans="1:4" ht="15.75">
       <c r="A11" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C11" t="b">
         <v>0</v>
@@ -2504,10 +2511,10 @@
     </row>
     <row r="12" spans="1:4" ht="15.75">
       <c r="A12" s="7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C12" t="b">
         <v>0</v>
@@ -2515,10 +2522,10 @@
     </row>
     <row r="13" spans="1:4" ht="15.75">
       <c r="A13" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C13" t="b">
         <v>0</v>
@@ -2526,10 +2533,10 @@
     </row>
     <row r="14" spans="1:4" ht="15.75">
       <c r="A14" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C14" t="b">
         <v>0</v>
@@ -2537,10 +2544,10 @@
     </row>
     <row r="15" spans="1:4" ht="15.75">
       <c r="A15" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C15" t="b">
         <v>0</v>
@@ -2548,10 +2555,10 @@
     </row>
     <row r="16" spans="1:4" ht="15.75">
       <c r="A16" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C16" t="b">
         <v>0</v>
@@ -2559,10 +2566,10 @@
     </row>
     <row r="17" spans="1:3" ht="15.75">
       <c r="A17" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C17" t="b">
         <v>0</v>
@@ -2570,10 +2577,10 @@
     </row>
     <row r="18" spans="1:3" ht="15.75">
       <c r="A18" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C18" t="b">
         <v>0</v>
@@ -2581,10 +2588,10 @@
     </row>
     <row r="19" spans="1:3" ht="15.75">
       <c r="A19" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C19" t="b">
         <v>0</v>
@@ -2592,10 +2599,10 @@
     </row>
     <row r="20" spans="1:3" ht="15.75">
       <c r="A20" s="7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C20" t="b">
         <v>0</v>
@@ -2603,10 +2610,10 @@
     </row>
     <row r="21" spans="1:3" ht="15.75">
       <c r="A21" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C21" t="b">
         <v>0</v>
@@ -2614,10 +2621,10 @@
     </row>
     <row r="22" spans="1:3" ht="15.75">
       <c r="A22" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C22" t="b">
         <v>0</v>
@@ -2625,10 +2632,10 @@
     </row>
     <row r="23" spans="1:3" ht="15.75">
       <c r="A23" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C23" t="b">
         <v>0</v>
@@ -2636,10 +2643,10 @@
     </row>
     <row r="24" spans="1:3" ht="15.75">
       <c r="A24" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C24" t="b">
         <v>0</v>
@@ -2647,10 +2654,10 @@
     </row>
     <row r="25" spans="1:3" ht="15.75">
       <c r="A25" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C25" t="b">
         <v>0</v>
@@ -2658,10 +2665,10 @@
     </row>
     <row r="26" spans="1:3" ht="15.75">
       <c r="A26" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C26" t="b">
         <v>0</v>
@@ -2669,10 +2676,10 @@
     </row>
     <row r="27" spans="1:3" ht="15.75">
       <c r="A27" s="7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C27" t="b">
         <v>0</v>
@@ -2680,10 +2687,10 @@
     </row>
     <row r="28" spans="1:3" ht="15.75">
       <c r="A28" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C28" t="b">
         <v>0</v>
@@ -2691,10 +2698,10 @@
     </row>
     <row r="29" spans="1:3" ht="15.75">
       <c r="A29" s="7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C29" t="b">
         <v>0</v>
@@ -2702,10 +2709,10 @@
     </row>
     <row r="30" spans="1:3" ht="15.75">
       <c r="A30" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C30" t="b">
         <v>0</v>
@@ -2713,10 +2720,10 @@
     </row>
     <row r="31" spans="1:3" ht="15.75">
       <c r="A31" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C31" t="b">
         <v>0</v>
@@ -2724,10 +2731,10 @@
     </row>
     <row r="32" spans="1:3" ht="15.75">
       <c r="A32" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C32" t="b">
         <v>0</v>
@@ -2735,10 +2742,10 @@
     </row>
     <row r="33" spans="1:3" ht="15.75">
       <c r="A33" s="7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C33" t="b">
         <v>0</v>
@@ -2746,10 +2753,10 @@
     </row>
     <row r="34" spans="1:3" ht="15.75">
       <c r="A34" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C34" t="b">
         <v>0</v>
@@ -2757,10 +2764,10 @@
     </row>
     <row r="35" spans="1:3" ht="15.75">
       <c r="A35" s="7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C35" t="b">
         <v>0</v>
@@ -2768,10 +2775,10 @@
     </row>
     <row r="36" spans="1:3" ht="15.75">
       <c r="A36" s="7" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C36" t="b">
         <v>0</v>
@@ -2779,10 +2786,10 @@
     </row>
     <row r="37" spans="1:3" ht="15.75">
       <c r="A37" s="7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C37" t="b">
         <v>0</v>
@@ -2790,10 +2797,10 @@
     </row>
     <row r="38" spans="1:3" ht="15.75">
       <c r="A38" s="7" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C38" t="b">
         <v>0</v>
@@ -2801,10 +2808,10 @@
     </row>
     <row r="39" spans="1:3" ht="15.75">
       <c r="A39" s="7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C39" t="b">
         <v>0</v>
@@ -2812,10 +2819,10 @@
     </row>
     <row r="40" spans="1:3" ht="15.75">
       <c r="A40" s="7" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C40" t="b">
         <v>0</v>
@@ -2823,10 +2830,10 @@
     </row>
     <row r="41" spans="1:3" ht="15.75">
       <c r="A41" s="7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C41" t="b">
         <v>0</v>
@@ -2834,10 +2841,10 @@
     </row>
     <row r="42" spans="1:3" ht="15.75">
       <c r="A42" s="7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C42" t="b">
         <v>0</v>
@@ -2845,10 +2852,10 @@
     </row>
     <row r="43" spans="1:3" ht="15.75">
       <c r="A43" s="7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C43" t="b">
         <v>0</v>
@@ -2856,10 +2863,10 @@
     </row>
     <row r="44" spans="1:3" ht="15.75">
       <c r="A44" s="7" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C44" t="b">
         <v>0</v>
@@ -2867,10 +2874,10 @@
     </row>
     <row r="45" spans="1:3" ht="15.75">
       <c r="A45" s="7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C45" t="b">
         <v>0</v>
@@ -2878,10 +2885,10 @@
     </row>
     <row r="46" spans="1:3" ht="15.75">
       <c r="A46" s="7" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C46" t="b">
         <v>0</v>
@@ -2889,10 +2896,10 @@
     </row>
     <row r="47" spans="1:3" ht="15.75">
       <c r="A47" s="7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C47" t="b">
         <v>0</v>
@@ -2900,10 +2907,10 @@
     </row>
     <row r="48" spans="1:3" ht="15.75">
       <c r="A48" s="7" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C48" t="b">
         <v>0</v>
@@ -2911,10 +2918,10 @@
     </row>
     <row r="49" spans="1:4" ht="15.75">
       <c r="A49" s="7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C49" t="b">
         <v>0</v>
@@ -2922,10 +2929,10 @@
     </row>
     <row r="50" spans="1:4" ht="15.75">
       <c r="A50" s="7" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C50" t="b">
         <v>0</v>
@@ -2933,10 +2940,10 @@
     </row>
     <row r="51" spans="1:4" ht="15.75">
       <c r="A51" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C51" t="b">
         <v>0</v>
@@ -2944,10 +2951,10 @@
     </row>
     <row r="52" spans="1:4" ht="15.75">
       <c r="A52" s="7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C52" t="b">
         <v>0</v>
@@ -2955,10 +2962,10 @@
     </row>
     <row r="53" spans="1:4" ht="15.75">
       <c r="A53" s="7" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C53" t="b">
         <v>0</v>
@@ -2966,10 +2973,10 @@
     </row>
     <row r="54" spans="1:4" ht="15.75">
       <c r="A54" s="7" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C54" t="b">
         <v>0</v>
@@ -2977,10 +2984,10 @@
     </row>
     <row r="55" spans="1:4" ht="15.75">
       <c r="A55" s="7" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C55" t="b">
         <v>0</v>
@@ -2988,10 +2995,10 @@
     </row>
     <row r="56" spans="1:4" ht="15.75">
       <c r="A56" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C56" t="b">
         <v>0</v>
@@ -2999,10 +3006,10 @@
     </row>
     <row r="57" spans="1:4" ht="15.75">
       <c r="A57" s="7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C57" t="b">
         <v>0</v>
@@ -3010,10 +3017,10 @@
     </row>
     <row r="58" spans="1:4" ht="15.75">
       <c r="A58" s="7" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C58" t="b">
         <v>0</v>
@@ -3021,10 +3028,10 @@
     </row>
     <row r="59" spans="1:4" ht="15.75">
       <c r="A59" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C59" t="b">
         <v>0</v>
@@ -3035,10 +3042,10 @@
     </row>
     <row r="60" spans="1:4" ht="15.75">
       <c r="A60" s="7" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C60" t="b">
         <v>0</v>
@@ -3046,10 +3053,10 @@
     </row>
     <row r="61" spans="1:4" ht="15.75">
       <c r="A61" s="7" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C61" t="b">
         <v>0</v>
@@ -3057,10 +3064,10 @@
     </row>
     <row r="62" spans="1:4" ht="15.75">
       <c r="A62" s="7" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C62" t="b">
         <v>0</v>
@@ -3068,10 +3075,10 @@
     </row>
     <row r="63" spans="1:4" ht="15.75">
       <c r="A63" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C63" t="b">
         <v>0</v>
@@ -3079,10 +3086,10 @@
     </row>
     <row r="64" spans="1:4" ht="15.75">
       <c r="A64" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C64" t="b">
         <v>0</v>
@@ -3090,10 +3097,10 @@
     </row>
     <row r="65" spans="1:4" ht="15.75">
       <c r="A65" s="7" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C65" t="b">
         <v>1</v>
@@ -3104,10 +3111,10 @@
     </row>
     <row r="66" spans="1:4" ht="15.75">
       <c r="A66" s="7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C66" t="b">
         <v>1</v>
@@ -3118,10 +3125,10 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B67" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C67" t="b">
         <v>1</v>
@@ -3132,10 +3139,10 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B68" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C68" t="b">
         <v>1</v>
@@ -3146,10 +3153,10 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B69" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C69" t="b">
         <v>1</v>
@@ -3160,10 +3167,10 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B70" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C70" t="b">
         <v>1</v>
@@ -3174,10 +3181,10 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B71" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C71" t="b">
         <v>1</v>
@@ -3188,10 +3195,10 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B72" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C72" t="b">
         <v>1</v>
@@ -3202,10 +3209,10 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B73" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C73" t="b">
         <v>1</v>
@@ -3216,10 +3223,10 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B74" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C74" t="b">
         <v>1</v>
@@ -3230,10 +3237,10 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B75" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C75" t="b">
         <v>1</v>
@@ -3244,10 +3251,10 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B76" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C76" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Code clean up, refactor and changes due to database updates
</commit_message>
<xml_diff>
--- a/resources/test_data_user.xlsx
+++ b/resources/test_data_user.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\OneDrive - UNSW\University\Postgraduate\Year 3 Trimester 3\COMP9900\Project\BackEnd\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB4E4241-484B-4190-B6C5-3DB455896D12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEEBD79C-ADAD-4160-845C-AC00DD97ADB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10605" yWindow="0" windowWidth="25650" windowHeight="21000" firstSheet="4" activeTab="5" xr2:uid="{1A28855D-1372-4992-8C97-28705A0C69E1}"/>
+    <workbookView xWindow="10605" yWindow="0" windowWidth="25650" windowHeight="21000" xr2:uid="{1A28855D-1372-4992-8C97-28705A0C69E1}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
@@ -1105,8 +1105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36BB9172-4BA3-48EB-851A-CC045B92290E}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1181,7 +1181,7 @@
       </c>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
@@ -1272,9 +1272,10 @@
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{73480234-B25F-499D-AC8A-F116F644BDCD}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{89A3B1A2-7428-49BF-BEBE-2C1D9A26B077}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1780,7 +1781,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{839B1F08-9FB4-4205-9D29-58AB9BDB11FE}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updating close_balance to $100k
</commit_message>
<xml_diff>
--- a/resources/test_data_user.xlsx
+++ b/resources/test_data_user.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\OneDrive - UNSW\University\Postgraduate\Year 3 Trimester 3\COMP9900\Project\BackEnd\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kovid\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEEBD79C-ADAD-4160-845C-AC00DD97ADB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9A37B07-89F1-4850-BFC8-4099FEA798EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10605" yWindow="0" windowWidth="25650" windowHeight="21000" xr2:uid="{1A28855D-1372-4992-8C97-28705A0C69E1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="4" xr2:uid="{1A28855D-1372-4992-8C97-28705A0C69E1}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
@@ -25,15 +25,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1105,7 +1096,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36BB9172-4BA3-48EB-851A-CC045B92290E}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1676,8 +1667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9448928-3915-4856-835A-5C489B392B12}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1709,7 +1700,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>10000</v>
+        <v>100000</v>
       </c>
       <c r="D2" s="7">
         <v>44119.108414351853</v>
@@ -1723,7 +1714,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>10000</v>
+        <v>100000</v>
       </c>
       <c r="D3" s="7">
         <v>44119.150081018517</v>
@@ -1737,7 +1728,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>10000</v>
+        <v>100000</v>
       </c>
       <c r="D4" s="7">
         <v>44119.191747685189</v>
@@ -1751,7 +1742,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>10000</v>
+        <v>100000</v>
       </c>
       <c r="D5" s="7">
         <v>44119.233414351853</v>
@@ -1765,7 +1756,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>10000</v>
+        <v>100000</v>
       </c>
       <c r="D6" s="7">
         <v>44119.275081018517</v>

</xml_diff>

<commit_message>
Added some tests, added fields to Portfolio and PortfolioPrice in db, made function to calculate the portfolio prices for all users. Need to make the function run with a scheduler. ToDo
</commit_message>
<xml_diff>
--- a/resources/test_data_user.xlsx
+++ b/resources/test_data_user.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kovid\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\OneDrive - UNSW\University\Postgraduate\Year 3 Trimester 3\COMP9900\Project\BackEnd\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9A37B07-89F1-4850-BFC8-4099FEA798EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F885800-0DA8-445D-A262-74387A52580F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="4" xr2:uid="{1A28855D-1372-4992-8C97-28705A0C69E1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13920" windowHeight="21000" firstSheet="3" activeTab="3" xr2:uid="{1A28855D-1372-4992-8C97-28705A0C69E1}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="205">
   <si>
     <t>j.meraachli@student.unsw.edu.au</t>
   </si>
@@ -206,9 +206,6 @@
     <t>portfolio</t>
   </si>
   <si>
-    <t>portfolio_price</t>
-  </si>
-  <si>
     <t>pass1234</t>
   </si>
   <si>
@@ -663,6 +660,12 @@
   </si>
   <si>
     <t>Ford</t>
+  </si>
+  <si>
+    <t>balance</t>
+  </si>
+  <si>
+    <t>investment_value</t>
   </si>
 </sst>
 </file>
@@ -1154,7 +1157,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -1176,7 +1179,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -1198,7 +1201,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
@@ -1220,7 +1223,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -1242,7 +1245,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6" t="s">
         <v>14</v>
@@ -1293,7 +1296,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1326,7 +1329,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1334,7 +1337,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -1354,7 +1357,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -1364,7 +1367,7 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -1383,7 +1386,7 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E12" s="3"/>
     </row>
@@ -1410,7 +1413,7 @@
         <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1466,7 +1469,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B2" t="s">
         <v>33</v>
@@ -1546,10 +1549,10 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
+        <v>200</v>
+      </c>
+      <c r="B6" t="s">
         <v>201</v>
-      </c>
-      <c r="B6" t="s">
-        <v>202</v>
       </c>
       <c r="C6" t="s">
         <v>35</v>
@@ -1566,10 +1569,10 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C7" t="s">
         <v>35</v>
@@ -1591,20 +1594,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51161AFF-7779-4BC8-A52D-606E943847CF}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -1612,50 +1614,62 @@
         <v>40</v>
       </c>
       <c r="C1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>52</v>
+      </c>
+      <c r="C2">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>53</v>
+      </c>
+      <c r="C3">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>54</v>
+      </c>
+      <c r="C4">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>55</v>
+      </c>
+      <c r="C5">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>56</v>
+      </c>
+      <c r="C6">
+        <v>100000</v>
       </c>
     </row>
   </sheetData>
@@ -1665,20 +1679,21 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9448928-3915-4856-835A-5C489B392B12}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -1689,10 +1704,13 @@
         <v>41</v>
       </c>
       <c r="D1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1702,11 +1720,14 @@
       <c r="C2">
         <v>100000</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="7">
         <v>44119.108414351853</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1716,11 +1737,14 @@
       <c r="C3">
         <v>100000</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="7">
         <v>44119.150081018517</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1730,11 +1754,14 @@
       <c r="C4">
         <v>100000</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="7">
         <v>44119.191747685189</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1744,11 +1771,14 @@
       <c r="C5">
         <v>100000</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="7">
         <v>44119.233414351853</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1758,7 +1788,10 @@
       <c r="C6">
         <v>100000</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" s="7">
         <v>44119.275081018517</v>
       </c>
     </row>
@@ -1793,7 +1826,7 @@
         <v>26</v>
       </c>
       <c r="D1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E1" t="s">
         <v>42</v>
@@ -1813,7 +1846,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D2">
         <v>10</v>
@@ -1882,7 +1915,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D5">
         <v>40</v>
@@ -1905,7 +1938,7 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D6">
         <v>10</v>
@@ -1974,7 +2007,7 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D9">
         <v>40</v>
@@ -2020,7 +2053,7 @@
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D11">
         <v>60</v>
@@ -2069,24 +2102,24 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75">
       <c r="A1" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75">
       <c r="A2" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>60</v>
       </c>
       <c r="C2" t="b">
         <v>0</v>
@@ -2094,10 +2127,10 @@
     </row>
     <row r="3" spans="1:4" ht="15.75">
       <c r="A3" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>61</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>62</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
@@ -2105,10 +2138,10 @@
     </row>
     <row r="4" spans="1:4" ht="15.75">
       <c r="A4" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>63</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>64</v>
       </c>
       <c r="C4" t="b">
         <v>0</v>
@@ -2116,10 +2149,10 @@
     </row>
     <row r="5" spans="1:4" ht="15.75">
       <c r="A5" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>65</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>66</v>
       </c>
       <c r="C5" t="b">
         <v>0</v>
@@ -2127,10 +2160,10 @@
     </row>
     <row r="6" spans="1:4" ht="15.75">
       <c r="A6" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>67</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>68</v>
       </c>
       <c r="C6" t="b">
         <v>0</v>
@@ -2138,10 +2171,10 @@
     </row>
     <row r="7" spans="1:4" ht="15.75">
       <c r="A7" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>69</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>70</v>
       </c>
       <c r="C7" t="b">
         <v>0</v>
@@ -2149,10 +2182,10 @@
     </row>
     <row r="8" spans="1:4" ht="15.75">
       <c r="A8" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>71</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>72</v>
       </c>
       <c r="C8" t="b">
         <v>0</v>
@@ -2160,10 +2193,10 @@
     </row>
     <row r="9" spans="1:4" ht="15.75">
       <c r="A9" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>73</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>74</v>
       </c>
       <c r="C9" t="b">
         <v>0</v>
@@ -2171,10 +2204,10 @@
     </row>
     <row r="10" spans="1:4" ht="15.75">
       <c r="A10" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>75</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>76</v>
       </c>
       <c r="C10" t="b">
         <v>0</v>
@@ -2182,10 +2215,10 @@
     </row>
     <row r="11" spans="1:4" ht="15.75">
       <c r="A11" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>77</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>78</v>
       </c>
       <c r="C11" t="b">
         <v>0</v>
@@ -2193,10 +2226,10 @@
     </row>
     <row r="12" spans="1:4" ht="15.75">
       <c r="A12" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>79</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>80</v>
       </c>
       <c r="C12" t="b">
         <v>0</v>
@@ -2204,10 +2237,10 @@
     </row>
     <row r="13" spans="1:4" ht="15.75">
       <c r="A13" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" s="8" t="s">
         <v>81</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>82</v>
       </c>
       <c r="C13" t="b">
         <v>0</v>
@@ -2215,10 +2248,10 @@
     </row>
     <row r="14" spans="1:4" ht="15.75">
       <c r="A14" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" s="8" t="s">
         <v>83</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>84</v>
       </c>
       <c r="C14" t="b">
         <v>0</v>
@@ -2226,10 +2259,10 @@
     </row>
     <row r="15" spans="1:4" ht="15.75">
       <c r="A15" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15" s="8" t="s">
         <v>85</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>86</v>
       </c>
       <c r="C15" t="b">
         <v>0</v>
@@ -2237,10 +2270,10 @@
     </row>
     <row r="16" spans="1:4" ht="15.75">
       <c r="A16" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>87</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>88</v>
       </c>
       <c r="C16" t="b">
         <v>0</v>
@@ -2248,10 +2281,10 @@
     </row>
     <row r="17" spans="1:3" ht="15.75">
       <c r="A17" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>89</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>90</v>
       </c>
       <c r="C17" t="b">
         <v>0</v>
@@ -2259,10 +2292,10 @@
     </row>
     <row r="18" spans="1:3" ht="15.75">
       <c r="A18" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B18" s="8" t="s">
         <v>91</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>92</v>
       </c>
       <c r="C18" t="b">
         <v>0</v>
@@ -2270,10 +2303,10 @@
     </row>
     <row r="19" spans="1:3" ht="15.75">
       <c r="A19" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" s="8" t="s">
         <v>93</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>94</v>
       </c>
       <c r="C19" t="b">
         <v>0</v>
@@ -2281,10 +2314,10 @@
     </row>
     <row r="20" spans="1:3" ht="15.75">
       <c r="A20" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B20" s="8" t="s">
         <v>95</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>96</v>
       </c>
       <c r="C20" t="b">
         <v>0</v>
@@ -2292,10 +2325,10 @@
     </row>
     <row r="21" spans="1:3" ht="15.75">
       <c r="A21" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B21" s="8" t="s">
         <v>97</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>98</v>
       </c>
       <c r="C21" t="b">
         <v>0</v>
@@ -2303,10 +2336,10 @@
     </row>
     <row r="22" spans="1:3" ht="15.75">
       <c r="A22" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B22" s="8" t="s">
         <v>99</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>100</v>
       </c>
       <c r="C22" t="b">
         <v>0</v>
@@ -2314,10 +2347,10 @@
     </row>
     <row r="23" spans="1:3" ht="15.75">
       <c r="A23" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B23" s="8" t="s">
         <v>101</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>102</v>
       </c>
       <c r="C23" t="b">
         <v>0</v>
@@ -2325,10 +2358,10 @@
     </row>
     <row r="24" spans="1:3" ht="15.75">
       <c r="A24" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="B24" s="8" t="s">
         <v>103</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>104</v>
       </c>
       <c r="C24" t="b">
         <v>0</v>
@@ -2336,10 +2369,10 @@
     </row>
     <row r="25" spans="1:3" ht="15.75">
       <c r="A25" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B25" s="8" t="s">
         <v>105</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>106</v>
       </c>
       <c r="C25" t="b">
         <v>0</v>
@@ -2347,10 +2380,10 @@
     </row>
     <row r="26" spans="1:3" ht="15.75">
       <c r="A26" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B26" s="8" t="s">
         <v>107</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>108</v>
       </c>
       <c r="C26" t="b">
         <v>0</v>
@@ -2358,10 +2391,10 @@
     </row>
     <row r="27" spans="1:3" ht="15.75">
       <c r="A27" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B27" s="8" t="s">
         <v>109</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>110</v>
       </c>
       <c r="C27" t="b">
         <v>0</v>
@@ -2369,10 +2402,10 @@
     </row>
     <row r="28" spans="1:3" ht="15.75">
       <c r="A28" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B28" s="8" t="s">
         <v>111</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>112</v>
       </c>
       <c r="C28" t="b">
         <v>0</v>
@@ -2380,10 +2413,10 @@
     </row>
     <row r="29" spans="1:3" ht="15.75">
       <c r="A29" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B29" s="8" t="s">
         <v>113</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>114</v>
       </c>
       <c r="C29" t="b">
         <v>0</v>
@@ -2391,10 +2424,10 @@
     </row>
     <row r="30" spans="1:3" ht="15.75">
       <c r="A30" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B30" s="8" t="s">
         <v>115</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>116</v>
       </c>
       <c r="C30" t="b">
         <v>0</v>
@@ -2402,10 +2435,10 @@
     </row>
     <row r="31" spans="1:3" ht="15.75">
       <c r="A31" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B31" s="8" t="s">
         <v>117</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>118</v>
       </c>
       <c r="C31" t="b">
         <v>0</v>
@@ -2413,10 +2446,10 @@
     </row>
     <row r="32" spans="1:3" ht="15.75">
       <c r="A32" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B32" s="8" t="s">
         <v>119</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>120</v>
       </c>
       <c r="C32" t="b">
         <v>0</v>
@@ -2424,10 +2457,10 @@
     </row>
     <row r="33" spans="1:3" ht="15.75">
       <c r="A33" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="B33" s="8" t="s">
         <v>121</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>122</v>
       </c>
       <c r="C33" t="b">
         <v>0</v>
@@ -2435,10 +2468,10 @@
     </row>
     <row r="34" spans="1:3" ht="15.75">
       <c r="A34" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="B34" s="8" t="s">
         <v>123</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>124</v>
       </c>
       <c r="C34" t="b">
         <v>0</v>
@@ -2446,10 +2479,10 @@
     </row>
     <row r="35" spans="1:3" ht="15.75">
       <c r="A35" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B35" s="8" t="s">
         <v>125</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>126</v>
       </c>
       <c r="C35" t="b">
         <v>0</v>
@@ -2457,10 +2490,10 @@
     </row>
     <row r="36" spans="1:3" ht="15.75">
       <c r="A36" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B36" s="8" t="s">
         <v>127</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>128</v>
       </c>
       <c r="C36" t="b">
         <v>0</v>
@@ -2468,10 +2501,10 @@
     </row>
     <row r="37" spans="1:3" ht="15.75">
       <c r="A37" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="B37" s="8" t="s">
         <v>129</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>130</v>
       </c>
       <c r="C37" t="b">
         <v>0</v>
@@ -2479,10 +2512,10 @@
     </row>
     <row r="38" spans="1:3" ht="15.75">
       <c r="A38" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="B38" s="8" t="s">
         <v>131</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>132</v>
       </c>
       <c r="C38" t="b">
         <v>0</v>
@@ -2490,10 +2523,10 @@
     </row>
     <row r="39" spans="1:3" ht="15.75">
       <c r="A39" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="B39" s="8" t="s">
         <v>133</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>134</v>
       </c>
       <c r="C39" t="b">
         <v>0</v>
@@ -2501,10 +2534,10 @@
     </row>
     <row r="40" spans="1:3" ht="15.75">
       <c r="A40" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B40" s="8" t="s">
         <v>135</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>136</v>
       </c>
       <c r="C40" t="b">
         <v>0</v>
@@ -2512,10 +2545,10 @@
     </row>
     <row r="41" spans="1:3" ht="15.75">
       <c r="A41" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="B41" s="8" t="s">
         <v>137</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>138</v>
       </c>
       <c r="C41" t="b">
         <v>0</v>
@@ -2523,10 +2556,10 @@
     </row>
     <row r="42" spans="1:3" ht="15.75">
       <c r="A42" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="B42" s="8" t="s">
         <v>139</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>140</v>
       </c>
       <c r="C42" t="b">
         <v>0</v>
@@ -2534,10 +2567,10 @@
     </row>
     <row r="43" spans="1:3" ht="15.75">
       <c r="A43" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="B43" s="8" t="s">
         <v>141</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>142</v>
       </c>
       <c r="C43" t="b">
         <v>0</v>
@@ -2545,10 +2578,10 @@
     </row>
     <row r="44" spans="1:3" ht="15.75">
       <c r="A44" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="B44" s="8" t="s">
         <v>143</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>144</v>
       </c>
       <c r="C44" t="b">
         <v>0</v>
@@ -2556,10 +2589,10 @@
     </row>
     <row r="45" spans="1:3" ht="15.75">
       <c r="A45" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="B45" s="8" t="s">
         <v>145</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>146</v>
       </c>
       <c r="C45" t="b">
         <v>0</v>
@@ -2567,10 +2600,10 @@
     </row>
     <row r="46" spans="1:3" ht="15.75">
       <c r="A46" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="B46" s="8" t="s">
         <v>147</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>148</v>
       </c>
       <c r="C46" t="b">
         <v>0</v>
@@ -2578,10 +2611,10 @@
     </row>
     <row r="47" spans="1:3" ht="15.75">
       <c r="A47" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="B47" s="8" t="s">
         <v>149</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>150</v>
       </c>
       <c r="C47" t="b">
         <v>0</v>
@@ -2589,10 +2622,10 @@
     </row>
     <row r="48" spans="1:3" ht="15.75">
       <c r="A48" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="B48" s="8" t="s">
         <v>151</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>152</v>
       </c>
       <c r="C48" t="b">
         <v>0</v>
@@ -2600,10 +2633,10 @@
     </row>
     <row r="49" spans="1:4" ht="15.75">
       <c r="A49" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="B49" s="8" t="s">
         <v>153</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>154</v>
       </c>
       <c r="C49" t="b">
         <v>0</v>
@@ -2611,10 +2644,10 @@
     </row>
     <row r="50" spans="1:4" ht="15.75">
       <c r="A50" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="B50" s="8" t="s">
         <v>155</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>156</v>
       </c>
       <c r="C50" t="b">
         <v>0</v>
@@ -2622,10 +2655,10 @@
     </row>
     <row r="51" spans="1:4" ht="15.75">
       <c r="A51" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="B51" s="8" t="s">
         <v>157</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>158</v>
       </c>
       <c r="C51" t="b">
         <v>0</v>
@@ -2633,10 +2666,10 @@
     </row>
     <row r="52" spans="1:4" ht="15.75">
       <c r="A52" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="B52" s="8" t="s">
         <v>159</v>
-      </c>
-      <c r="B52" s="8" t="s">
-        <v>160</v>
       </c>
       <c r="C52" t="b">
         <v>0</v>
@@ -2644,10 +2677,10 @@
     </row>
     <row r="53" spans="1:4" ht="15.75">
       <c r="A53" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="B53" s="8" t="s">
         <v>161</v>
-      </c>
-      <c r="B53" s="8" t="s">
-        <v>162</v>
       </c>
       <c r="C53" t="b">
         <v>0</v>
@@ -2655,10 +2688,10 @@
     </row>
     <row r="54" spans="1:4" ht="15.75">
       <c r="A54" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="B54" s="8" t="s">
         <v>163</v>
-      </c>
-      <c r="B54" s="8" t="s">
-        <v>164</v>
       </c>
       <c r="C54" t="b">
         <v>0</v>
@@ -2666,10 +2699,10 @@
     </row>
     <row r="55" spans="1:4" ht="15.75">
       <c r="A55" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="B55" s="8" t="s">
         <v>165</v>
-      </c>
-      <c r="B55" s="8" t="s">
-        <v>166</v>
       </c>
       <c r="C55" t="b">
         <v>0</v>
@@ -2677,10 +2710,10 @@
     </row>
     <row r="56" spans="1:4" ht="15.75">
       <c r="A56" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="B56" s="8" t="s">
         <v>167</v>
-      </c>
-      <c r="B56" s="8" t="s">
-        <v>168</v>
       </c>
       <c r="C56" t="b">
         <v>0</v>
@@ -2688,10 +2721,10 @@
     </row>
     <row r="57" spans="1:4" ht="15.75">
       <c r="A57" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="B57" s="8" t="s">
         <v>169</v>
-      </c>
-      <c r="B57" s="8" t="s">
-        <v>170</v>
       </c>
       <c r="C57" t="b">
         <v>0</v>
@@ -2699,10 +2732,10 @@
     </row>
     <row r="58" spans="1:4" ht="15.75">
       <c r="A58" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="B58" s="8" t="s">
         <v>171</v>
-      </c>
-      <c r="B58" s="8" t="s">
-        <v>172</v>
       </c>
       <c r="C58" t="b">
         <v>0</v>
@@ -2710,10 +2743,10 @@
     </row>
     <row r="59" spans="1:4" ht="15.75">
       <c r="A59" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="B59" s="8" t="s">
         <v>173</v>
-      </c>
-      <c r="B59" s="8" t="s">
-        <v>174</v>
       </c>
       <c r="C59" t="b">
         <v>0</v>
@@ -2724,10 +2757,10 @@
     </row>
     <row r="60" spans="1:4" ht="15.75">
       <c r="A60" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="B60" s="8" t="s">
         <v>175</v>
-      </c>
-      <c r="B60" s="8" t="s">
-        <v>176</v>
       </c>
       <c r="C60" t="b">
         <v>0</v>
@@ -2735,10 +2768,10 @@
     </row>
     <row r="61" spans="1:4" ht="15.75">
       <c r="A61" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="B61" s="8" t="s">
         <v>177</v>
-      </c>
-      <c r="B61" s="8" t="s">
-        <v>178</v>
       </c>
       <c r="C61" t="b">
         <v>0</v>
@@ -2746,10 +2779,10 @@
     </row>
     <row r="62" spans="1:4" ht="15.75">
       <c r="A62" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="B62" s="8" t="s">
         <v>179</v>
-      </c>
-      <c r="B62" s="8" t="s">
-        <v>180</v>
       </c>
       <c r="C62" t="b">
         <v>0</v>
@@ -2757,10 +2790,10 @@
     </row>
     <row r="63" spans="1:4" ht="15.75">
       <c r="A63" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="B63" s="8" t="s">
         <v>181</v>
-      </c>
-      <c r="B63" s="8" t="s">
-        <v>182</v>
       </c>
       <c r="C63" t="b">
         <v>0</v>
@@ -2768,10 +2801,10 @@
     </row>
     <row r="64" spans="1:4" ht="15.75">
       <c r="A64" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="B64" s="8" t="s">
         <v>183</v>
-      </c>
-      <c r="B64" s="8" t="s">
-        <v>184</v>
       </c>
       <c r="C64" t="b">
         <v>0</v>
@@ -2782,10 +2815,10 @@
     </row>
     <row r="65" spans="1:4" ht="15.75">
       <c r="A65" s="8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C65" t="b">
         <v>1</v>
@@ -2796,10 +2829,10 @@
     </row>
     <row r="66" spans="1:4" ht="15.75">
       <c r="A66" s="8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C66" t="b">
         <v>1</v>
@@ -2810,10 +2843,10 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B67" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C67" t="b">
         <v>1</v>
@@ -2824,10 +2857,10 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B68" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C68" t="b">
         <v>1</v>
@@ -2838,10 +2871,10 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B69" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C69" t="b">
         <v>1</v>
@@ -2852,10 +2885,10 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B70" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C70" t="b">
         <v>1</v>
@@ -2866,10 +2899,10 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B71" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C71" t="b">
         <v>1</v>
@@ -2880,10 +2913,10 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B72" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C72" t="b">
         <v>1</v>
@@ -2894,10 +2927,10 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B73" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C73" t="b">
         <v>1</v>
@@ -2908,10 +2941,10 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B74" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C74" t="b">
         <v>1</v>
@@ -2922,10 +2955,10 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B75" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C75" t="b">
         <v>1</v>
@@ -2936,10 +2969,10 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B76" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C76" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Adding a Tester profile
</commit_message>
<xml_diff>
--- a/resources/test_data_user.xlsx
+++ b/resources/test_data_user.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\OneDrive - UNSW\University\Postgraduate\Year 3 Trimester 3\COMP9900\Project\BackEnd\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kovid\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F885800-0DA8-445D-A262-74387A52580F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3369B7D5-2EAB-4186-80D2-106C032EF9E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13920" windowHeight="21000" firstSheet="3" activeTab="3" xr2:uid="{1A28855D-1372-4992-8C97-28705A0C69E1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="6" xr2:uid="{1A28855D-1372-4992-8C97-28705A0C69E1}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="209">
   <si>
     <t>j.meraachli@student.unsw.edu.au</t>
   </si>
@@ -666,6 +666,18 @@
   </si>
   <si>
     <t>investment_value</t>
+  </si>
+  <si>
+    <t>test@test.com</t>
+  </si>
+  <si>
+    <t>Tester</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Tester's Portfolio</t>
   </si>
 </sst>
 </file>
@@ -1097,10 +1109,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36BB9172-4BA3-48EB-851A-CC045B92290E}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1262,23 +1274,44 @@
         <v>24</v>
       </c>
     </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B7">
+        <v>12345678</v>
+      </c>
+      <c r="C7" t="s">
+        <v>206</v>
+      </c>
+      <c r="D7" t="s">
+        <v>207</v>
+      </c>
+      <c r="G7" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{73480234-B25F-499D-AC8A-F116F644BDCD}"/>
     <hyperlink ref="A3" r:id="rId2" xr:uid="{89A3B1A2-7428-49BF-BEBE-2C1D9A26B077}"/>
+    <hyperlink ref="A7" r:id="rId3" xr:uid="{CFF3AA8F-27DF-4B79-9989-0EBAA5A65C47}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF8D5324-5018-9640-9915-418B2F181888}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -1429,6 +1462,38 @@
         <v>5</v>
       </c>
       <c r="B17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18">
+        <v>6</v>
+      </c>
+      <c r="B18" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20">
+        <v>6</v>
+      </c>
+      <c r="B20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21">
+        <v>6</v>
+      </c>
+      <c r="B21" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1594,10 +1659,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51161AFF-7779-4BC8-A52D-606E943847CF}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1672,6 +1737,17 @@
         <v>100000</v>
       </c>
     </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>208</v>
+      </c>
+      <c r="C7">
+        <v>1000000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1679,10 +1755,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9448928-3915-4856-835A-5C489B392B12}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1795,6 +1871,23 @@
         <v>44119.275081018517</v>
       </c>
     </row>
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>1000000</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" s="7">
+        <v>44120.275080960651</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1806,7 +1899,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2069,10 +2162,50 @@
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="E12" s="7"/>
+      <c r="A12">
+        <v>6</v>
+      </c>
+      <c r="B12">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12">
+        <v>60</v>
+      </c>
+      <c r="E12" s="7">
+        <v>44119.483414351853</v>
+      </c>
+      <c r="F12">
+        <v>2310</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="E13" s="7"/>
+      <c r="A13">
+        <v>6</v>
+      </c>
+      <c r="B13">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>200</v>
+      </c>
+      <c r="D13">
+        <v>60</v>
+      </c>
+      <c r="E13" s="7">
+        <v>44119.483414351853</v>
+      </c>
+      <c r="F13">
+        <v>3420</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:7">
       <c r="E14" s="7"/>
@@ -2090,7 +2223,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB0AE7CC-0281-42AB-BEFB-FF7CDAA66D40}">
   <dimension ref="A1:D76"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
       <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>

</xml_diff>